<commit_message>
added data processing code
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Excel/Balance-sheet_combined.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Excel/Balance-sheet_combined.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\OneDrive\Desktop\Kishan\Contractzy\WebScrapping\Tutorial\Financial_Data\MoneyControl\Companies\IT Services &amp; Consulting\3i Infotech Ltd\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBA4826-55D9-4F06-8938-4AE835F83AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1927,8 +1933,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1991,13 +1997,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2035,7 +2049,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2069,6 +2083,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2103,9 +2118,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2278,14 +2294,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2350,7 +2371,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -2412,17 +2433,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2508,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2552,7 +2573,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2617,7 +2638,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2682,7 +2703,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2747,12 +2768,12 @@
         <v>613</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2817,7 +2838,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2882,7 +2903,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2947,7 +2968,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -3012,7 +3033,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3077,12 +3098,12 @@
         <v>617</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -3147,7 +3168,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -3212,7 +3233,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3277,7 +3298,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3342,7 +3363,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -3407,7 +3428,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -3472,17 +3493,17 @@
         <v>623</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -3547,7 +3568,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -3612,7 +3633,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -3677,7 +3698,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3742,7 +3763,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -3807,7 +3828,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -3872,7 +3893,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -3937,7 +3958,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -4002,7 +4023,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -4067,7 +4088,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -4132,12 +4153,12 @@
         <v>629</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -4202,7 +4223,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -4267,7 +4288,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -4332,7 +4353,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -4397,7 +4418,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -4462,7 +4483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -4527,7 +4548,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -4592,7 +4613,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -4657,17 +4678,17 @@
         <v>623</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -4732,12 +4753,12 @@
         <v>634</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -4802,7 +4823,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -4867,7 +4888,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -4932,7 +4953,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>69</v>
       </c>
@@ -4997,12 +5018,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -5067,12 +5088,12 @@
         <v>550</v>
       </c>
     </row>
-    <row r="54" spans="1:21">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -5137,12 +5158,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:21">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:21">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -5207,7 +5228,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:21">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -5272,12 +5293,12 @@
         <v>635</v>
       </c>
     </row>
-    <row r="59" spans="1:21">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:21">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -5342,12 +5363,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:21">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -5412,7 +5433,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -5477,12 +5498,12 @@
         <v>627</v>
       </c>
     </row>
-    <row r="64" spans="1:21">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:21">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -5547,7 +5568,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:21">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>84</v>
       </c>

</xml_diff>